<commit_message>
fix(ui): evita loop infinito no carregamento de dados - Trata retorno 'false' na lógica de carregamento em BI_Giro_Status.py. - Corrige falha na interface que causava travamento quando a lista de produtos vinha vazia.
</commit_message>
<xml_diff>
--- a/OUTPUT/BI_ABASTECIMENTO/BONUS_CONT.xlsx
+++ b/OUTPUT/BI_ABASTECIMENTO/BONUS_CONT.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,31 +451,31 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46024</v>
+        <v>46030</v>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45989</v>
+        <v>46029</v>
       </c>
       <c r="B3" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45988</v>
+        <v>46028</v>
       </c>
       <c r="B4" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45987</v>
+        <v>46027</v>
       </c>
       <c r="B5" t="n">
         <v>33</v>
@@ -483,87 +483,87 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45986</v>
+        <v>46024</v>
       </c>
       <c r="B6" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45985</v>
+        <v>45989</v>
       </c>
       <c r="B7" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45983</v>
+        <v>45988</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45982</v>
+        <v>45987</v>
       </c>
       <c r="B9" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B10" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B11" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45978</v>
+        <v>45983</v>
       </c>
       <c r="B12" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45975</v>
+        <v>45982</v>
       </c>
       <c r="B13" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B14" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B15" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B16" t="n">
         <v>29</v>
@@ -571,143 +571,143 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45971</v>
+        <v>45975</v>
       </c>
       <c r="B17" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45968</v>
+        <v>45974</v>
       </c>
       <c r="B18" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45967</v>
+        <v>45973</v>
       </c>
       <c r="B19" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45966</v>
+        <v>45972</v>
       </c>
       <c r="B20" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45965</v>
+        <v>45971</v>
       </c>
       <c r="B21" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45964</v>
+        <v>45968</v>
       </c>
       <c r="B22" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45961</v>
+        <v>45967</v>
       </c>
       <c r="B23" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45960</v>
+        <v>45966</v>
       </c>
       <c r="B24" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45959</v>
+        <v>45965</v>
       </c>
       <c r="B25" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45958</v>
+        <v>45964</v>
       </c>
       <c r="B26" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45957</v>
+        <v>45961</v>
       </c>
       <c r="B27" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45955</v>
+        <v>45960</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45954</v>
+        <v>45959</v>
       </c>
       <c r="B29" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45953</v>
+        <v>45958</v>
       </c>
       <c r="B30" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45952</v>
+        <v>45957</v>
       </c>
       <c r="B31" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45951</v>
+        <v>45955</v>
       </c>
       <c r="B32" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45950</v>
+        <v>45954</v>
       </c>
       <c r="B33" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45947</v>
+        <v>45953</v>
       </c>
       <c r="B34" t="n">
         <v>31</v>
@@ -715,135 +715,135 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45946</v>
+        <v>45952</v>
       </c>
       <c r="B35" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45945</v>
+        <v>45951</v>
       </c>
       <c r="B36" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45944</v>
+        <v>45950</v>
       </c>
       <c r="B37" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45943</v>
+        <v>45947</v>
       </c>
       <c r="B38" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45940</v>
+        <v>45946</v>
       </c>
       <c r="B39" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45939</v>
+        <v>45945</v>
       </c>
       <c r="B40" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45938</v>
+        <v>45944</v>
       </c>
       <c r="B41" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45937</v>
+        <v>45943</v>
       </c>
       <c r="B42" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45936</v>
+        <v>45940</v>
       </c>
       <c r="B43" t="n">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45933</v>
+        <v>45939</v>
       </c>
       <c r="B44" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45932</v>
+        <v>45938</v>
       </c>
       <c r="B45" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45931</v>
+        <v>45937</v>
       </c>
       <c r="B46" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45930</v>
+        <v>45936</v>
       </c>
       <c r="B47" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45929</v>
+        <v>45933</v>
       </c>
       <c r="B48" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45927</v>
+        <v>45932</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45926</v>
+        <v>45931</v>
       </c>
       <c r="B50" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45925</v>
+        <v>45930</v>
       </c>
       <c r="B51" t="n">
         <v>31</v>
@@ -851,471 +851,471 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45924</v>
+        <v>45929</v>
       </c>
       <c r="B52" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45923</v>
+        <v>45927</v>
       </c>
       <c r="B53" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45922</v>
+        <v>45926</v>
       </c>
       <c r="B54" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45919</v>
+        <v>45925</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45918</v>
+        <v>45924</v>
       </c>
       <c r="B56" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45917</v>
+        <v>45923</v>
       </c>
       <c r="B57" t="n">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45916</v>
+        <v>45922</v>
       </c>
       <c r="B58" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45915</v>
+        <v>45919</v>
       </c>
       <c r="B59" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45912</v>
+        <v>45918</v>
       </c>
       <c r="B60" t="n">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45911</v>
+        <v>45917</v>
       </c>
       <c r="B61" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45910</v>
+        <v>45916</v>
       </c>
       <c r="B62" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45909</v>
+        <v>45915</v>
       </c>
       <c r="B63" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45908</v>
+        <v>45912</v>
       </c>
       <c r="B64" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45905</v>
+        <v>45911</v>
       </c>
       <c r="B65" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45904</v>
+        <v>45910</v>
       </c>
       <c r="B66" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45903</v>
+        <v>45909</v>
       </c>
       <c r="B67" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45902</v>
+        <v>45908</v>
       </c>
       <c r="B68" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45901</v>
+        <v>45905</v>
       </c>
       <c r="B69" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45898</v>
+        <v>45904</v>
       </c>
       <c r="B70" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45897</v>
+        <v>45903</v>
       </c>
       <c r="B71" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45896</v>
+        <v>45902</v>
       </c>
       <c r="B72" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45895</v>
+        <v>45901</v>
       </c>
       <c r="B73" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45894</v>
+        <v>45898</v>
       </c>
       <c r="B74" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45891</v>
+        <v>45897</v>
       </c>
       <c r="B75" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45890</v>
+        <v>45896</v>
       </c>
       <c r="B76" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45889</v>
+        <v>45895</v>
       </c>
       <c r="B77" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45888</v>
+        <v>45894</v>
       </c>
       <c r="B78" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45887</v>
+        <v>45891</v>
       </c>
       <c r="B79" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45884</v>
+        <v>45890</v>
       </c>
       <c r="B80" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45883</v>
+        <v>45889</v>
       </c>
       <c r="B81" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45882</v>
+        <v>45888</v>
       </c>
       <c r="B82" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>45881</v>
+        <v>45887</v>
       </c>
       <c r="B83" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>45880</v>
+        <v>45884</v>
       </c>
       <c r="B84" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>45877</v>
+        <v>45883</v>
       </c>
       <c r="B85" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45876</v>
+        <v>45882</v>
       </c>
       <c r="B86" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45875</v>
+        <v>45881</v>
       </c>
       <c r="B87" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45874</v>
+        <v>45880</v>
       </c>
       <c r="B88" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45873</v>
+        <v>45877</v>
       </c>
       <c r="B89" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45871</v>
+        <v>45876</v>
       </c>
       <c r="B90" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45870</v>
+        <v>45875</v>
       </c>
       <c r="B91" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45869</v>
+        <v>45874</v>
       </c>
       <c r="B92" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>45868</v>
+        <v>45873</v>
       </c>
       <c r="B93" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>45867</v>
+        <v>45871</v>
       </c>
       <c r="B94" t="n">
-        <v>41</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>45866</v>
+        <v>45870</v>
       </c>
       <c r="B95" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>45864</v>
+        <v>45869</v>
       </c>
       <c r="B96" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>45863</v>
+        <v>45868</v>
       </c>
       <c r="B97" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>45862</v>
+        <v>45867</v>
       </c>
       <c r="B98" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>45861</v>
+        <v>45866</v>
       </c>
       <c r="B99" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>45860</v>
+        <v>45864</v>
       </c>
       <c r="B100" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>45859</v>
+        <v>45863</v>
       </c>
       <c r="B101" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>45857</v>
+        <v>45862</v>
       </c>
       <c r="B102" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>45856</v>
+        <v>45861</v>
       </c>
       <c r="B103" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>45855</v>
+        <v>45860</v>
       </c>
       <c r="B104" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>45854</v>
+        <v>45859</v>
       </c>
       <c r="B105" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>45853</v>
+        <v>45857</v>
       </c>
       <c r="B106" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>45852</v>
+        <v>45856</v>
       </c>
       <c r="B107" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>45849</v>
+        <v>45855</v>
       </c>
       <c r="B108" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>45848</v>
+        <v>45854</v>
       </c>
       <c r="B109" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>45847</v>
+        <v>45853</v>
       </c>
       <c r="B110" t="n">
         <v>35</v>
@@ -1323,441 +1323,473 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>45846</v>
+        <v>45852</v>
       </c>
       <c r="B111" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45845</v>
+        <v>45849</v>
       </c>
       <c r="B112" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>45843</v>
+        <v>45848</v>
       </c>
       <c r="B113" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>45842</v>
+        <v>45847</v>
       </c>
       <c r="B114" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>45841</v>
+        <v>45846</v>
       </c>
       <c r="B115" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>45840</v>
+        <v>45845</v>
       </c>
       <c r="B116" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45839</v>
+        <v>45843</v>
       </c>
       <c r="B117" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>45838</v>
+        <v>45842</v>
       </c>
       <c r="B118" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>45835</v>
+        <v>45841</v>
       </c>
       <c r="B119" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>45834</v>
+        <v>45840</v>
       </c>
       <c r="B120" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>45833</v>
+        <v>45839</v>
       </c>
       <c r="B121" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>45832</v>
+        <v>45838</v>
       </c>
       <c r="B122" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>45831</v>
+        <v>45835</v>
       </c>
       <c r="B123" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>45829</v>
+        <v>45834</v>
       </c>
       <c r="B124" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>45828</v>
+        <v>45833</v>
       </c>
       <c r="B125" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>45827</v>
+        <v>45832</v>
       </c>
       <c r="B126" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>45826</v>
+        <v>45831</v>
       </c>
       <c r="B127" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>45825</v>
+        <v>45829</v>
       </c>
       <c r="B128" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>45824</v>
+        <v>45828</v>
       </c>
       <c r="B129" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>45822</v>
+        <v>45827</v>
       </c>
       <c r="B130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>45821</v>
+        <v>45826</v>
       </c>
       <c r="B131" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>45820</v>
+        <v>45825</v>
       </c>
       <c r="B132" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>45819</v>
+        <v>45824</v>
       </c>
       <c r="B133" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>45818</v>
+        <v>45822</v>
       </c>
       <c r="B134" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>45817</v>
+        <v>45821</v>
       </c>
       <c r="B135" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>45815</v>
+        <v>45820</v>
       </c>
       <c r="B136" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>45814</v>
+        <v>45819</v>
       </c>
       <c r="B137" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>45813</v>
+        <v>45818</v>
       </c>
       <c r="B138" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>45812</v>
+        <v>45817</v>
       </c>
       <c r="B139" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>45811</v>
+        <v>45815</v>
       </c>
       <c r="B140" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>45810</v>
+        <v>45814</v>
       </c>
       <c r="B141" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>45808</v>
+        <v>45813</v>
       </c>
       <c r="B142" t="n">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>45807</v>
+        <v>45812</v>
       </c>
       <c r="B143" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>45806</v>
+        <v>45811</v>
       </c>
       <c r="B144" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>45805</v>
+        <v>45810</v>
       </c>
       <c r="B145" t="n">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>45804</v>
+        <v>45808</v>
       </c>
       <c r="B146" t="n">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>45803</v>
+        <v>45807</v>
       </c>
       <c r="B147" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>45801</v>
+        <v>45806</v>
       </c>
       <c r="B148" t="n">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>45800</v>
+        <v>45805</v>
       </c>
       <c r="B149" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>45799</v>
+        <v>45804</v>
       </c>
       <c r="B150" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>45798</v>
+        <v>45803</v>
       </c>
       <c r="B151" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>45797</v>
+        <v>45801</v>
       </c>
       <c r="B152" t="n">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>45796</v>
+        <v>45800</v>
       </c>
       <c r="B153" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>45793</v>
+        <v>45799</v>
       </c>
       <c r="B154" t="n">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>45792</v>
+        <v>45798</v>
       </c>
       <c r="B155" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>45791</v>
+        <v>45797</v>
       </c>
       <c r="B156" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>45790</v>
+        <v>45796</v>
       </c>
       <c r="B157" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>45789</v>
+        <v>45793</v>
       </c>
       <c r="B158" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>45786</v>
+        <v>45792</v>
       </c>
       <c r="B159" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45785</v>
+        <v>45791</v>
       </c>
       <c r="B160" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45784</v>
+        <v>45790</v>
       </c>
       <c r="B161" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>45783</v>
+        <v>45789</v>
       </c>
       <c r="B162" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>45782</v>
+        <v>45786</v>
       </c>
       <c r="B163" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>45779</v>
+        <v>45785</v>
       </c>
       <c r="B164" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B165" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B166" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45782</v>
+      </c>
+      <c r="B167" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>45779</v>
+      </c>
+      <c r="B168" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
         <v>45778</v>
       </c>
-      <c r="B165" t="n">
+      <c r="B169" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
perf(pipeline): otimiza processamento e reduz tempo de cálculo - Substituído o uso de funções lambda no groupby por métodos nativos do Pandas. - Especificados 'engine' e 'usecols' na extração para reduzir o consumo de memória. - Corrigido o congelamento do script durante a execução da função pipeline(). - Preparado terreno para implementação de filtro temporal (limitação de 60/90 dias).
</commit_message>
<xml_diff>
--- a/OUTPUT/BI_ABASTECIMENTO/BONUS_CONT.xlsx
+++ b/OUTPUT/BI_ABASTECIMENTO/BONUS_CONT.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B169"/>
+  <dimension ref="A1:B170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,47 +451,47 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="B2" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46027</v>
+        <v>46028</v>
       </c>
       <c r="B5" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46024</v>
+        <v>46027</v>
       </c>
       <c r="B6" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45989</v>
+        <v>46024</v>
       </c>
       <c r="B7" t="n">
         <v>32</v>
@@ -499,95 +499,95 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B8" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45987</v>
+        <v>45988</v>
       </c>
       <c r="B9" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="B10" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="B11" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45983</v>
+        <v>45985</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45982</v>
+        <v>45983</v>
       </c>
       <c r="B13" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45980</v>
+        <v>45982</v>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="B15" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="B16" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="B17" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B18" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B19" t="n">
         <v>30</v>
@@ -595,119 +595,119 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B20" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B21" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="B22" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B23" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="B24" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45965</v>
+        <v>45966</v>
       </c>
       <c r="B25" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45964</v>
+        <v>45965</v>
       </c>
       <c r="B26" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45961</v>
+        <v>45964</v>
       </c>
       <c r="B27" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B28" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B29" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B30" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45957</v>
+        <v>45958</v>
       </c>
       <c r="B31" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45955</v>
+        <v>45957</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45954</v>
+        <v>45955</v>
       </c>
       <c r="B33" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B34" t="n">
         <v>31</v>
@@ -715,55 +715,55 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45952</v>
+        <v>45953</v>
       </c>
       <c r="B35" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45951</v>
+        <v>45952</v>
       </c>
       <c r="B36" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45950</v>
+        <v>45951</v>
       </c>
       <c r="B37" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45947</v>
+        <v>45950</v>
       </c>
       <c r="B38" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="B39" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B40" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45944</v>
+        <v>45945</v>
       </c>
       <c r="B41" t="n">
         <v>37</v>
@@ -771,47 +771,47 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45943</v>
+        <v>45944</v>
       </c>
       <c r="B42" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45940</v>
+        <v>45943</v>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45939</v>
+        <v>45940</v>
       </c>
       <c r="B44" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45938</v>
+        <v>45939</v>
       </c>
       <c r="B45" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45937</v>
+        <v>45938</v>
       </c>
       <c r="B46" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45936</v>
+        <v>45937</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -819,135 +819,135 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45933</v>
+        <v>45936</v>
       </c>
       <c r="B48" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45932</v>
+        <v>45933</v>
       </c>
       <c r="B49" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45931</v>
+        <v>45932</v>
       </c>
       <c r="B50" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45930</v>
+        <v>45931</v>
       </c>
       <c r="B51" t="n">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45929</v>
+        <v>45930</v>
       </c>
       <c r="B52" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45927</v>
+        <v>45929</v>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45926</v>
+        <v>45927</v>
       </c>
       <c r="B54" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B55" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B56" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B57" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B58" t="n">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45919</v>
+        <v>45922</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B60" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45917</v>
+        <v>45918</v>
       </c>
       <c r="B61" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45916</v>
+        <v>45917</v>
       </c>
       <c r="B62" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45915</v>
+        <v>45916</v>
       </c>
       <c r="B63" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45912</v>
+        <v>45915</v>
       </c>
       <c r="B64" t="n">
         <v>31</v>
@@ -955,223 +955,223 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="B65" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45910</v>
+        <v>45911</v>
       </c>
       <c r="B66" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45909</v>
+        <v>45910</v>
       </c>
       <c r="B67" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45908</v>
+        <v>45909</v>
       </c>
       <c r="B68" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45905</v>
+        <v>45908</v>
       </c>
       <c r="B69" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45904</v>
+        <v>45905</v>
       </c>
       <c r="B70" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45903</v>
+        <v>45904</v>
       </c>
       <c r="B71" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45902</v>
+        <v>45903</v>
       </c>
       <c r="B72" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45901</v>
+        <v>45902</v>
       </c>
       <c r="B73" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45898</v>
+        <v>45901</v>
       </c>
       <c r="B74" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45897</v>
+        <v>45898</v>
       </c>
       <c r="B75" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B76" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B77" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B78" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45891</v>
+        <v>45894</v>
       </c>
       <c r="B79" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B80" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B81" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45888</v>
+        <v>45889</v>
       </c>
       <c r="B82" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>45887</v>
+        <v>45888</v>
       </c>
       <c r="B83" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>45884</v>
+        <v>45887</v>
       </c>
       <c r="B84" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>45883</v>
+        <v>45884</v>
       </c>
       <c r="B85" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45882</v>
+        <v>45883</v>
       </c>
       <c r="B86" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="B87" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45880</v>
+        <v>45881</v>
       </c>
       <c r="B88" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45877</v>
+        <v>45880</v>
       </c>
       <c r="B89" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45876</v>
+        <v>45877</v>
       </c>
       <c r="B90" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45875</v>
+        <v>45876</v>
       </c>
       <c r="B91" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45874</v>
+        <v>45875</v>
       </c>
       <c r="B92" t="n">
         <v>19</v>
@@ -1179,31 +1179,31 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="B93" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>45871</v>
+        <v>45873</v>
       </c>
       <c r="B94" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>45870</v>
+        <v>45871</v>
       </c>
       <c r="B95" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>45869</v>
+        <v>45870</v>
       </c>
       <c r="B96" t="n">
         <v>31</v>
@@ -1211,119 +1211,119 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>45868</v>
+        <v>45869</v>
       </c>
       <c r="B97" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>45867</v>
+        <v>45868</v>
       </c>
       <c r="B98" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>45866</v>
+        <v>45867</v>
       </c>
       <c r="B99" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>45864</v>
+        <v>45866</v>
       </c>
       <c r="B100" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>45863</v>
+        <v>45864</v>
       </c>
       <c r="B101" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>45862</v>
+        <v>45863</v>
       </c>
       <c r="B102" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>45861</v>
+        <v>45862</v>
       </c>
       <c r="B103" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>45860</v>
+        <v>45861</v>
       </c>
       <c r="B104" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>45859</v>
+        <v>45860</v>
       </c>
       <c r="B105" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>45857</v>
+        <v>45859</v>
       </c>
       <c r="B106" t="n">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>45856</v>
+        <v>45857</v>
       </c>
       <c r="B107" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>45855</v>
+        <v>45856</v>
       </c>
       <c r="B108" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>45854</v>
+        <v>45855</v>
       </c>
       <c r="B109" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>45853</v>
+        <v>45854</v>
       </c>
       <c r="B110" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>45852</v>
+        <v>45853</v>
       </c>
       <c r="B111" t="n">
         <v>35</v>
@@ -1331,79 +1331,79 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45849</v>
+        <v>45852</v>
       </c>
       <c r="B112" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>45848</v>
+        <v>45849</v>
       </c>
       <c r="B113" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="B114" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B115" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B116" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45843</v>
+        <v>45845</v>
       </c>
       <c r="B117" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>45842</v>
+        <v>45843</v>
       </c>
       <c r="B118" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>45841</v>
+        <v>45842</v>
       </c>
       <c r="B119" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>45840</v>
+        <v>45841</v>
       </c>
       <c r="B120" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>45839</v>
+        <v>45840</v>
       </c>
       <c r="B121" t="n">
         <v>42</v>
@@ -1411,31 +1411,31 @@
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="B122" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>45835</v>
+        <v>45838</v>
       </c>
       <c r="B123" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="B124" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="B125" t="n">
         <v>33</v>
@@ -1443,255 +1443,255 @@
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>45832</v>
+        <v>45833</v>
       </c>
       <c r="B126" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>45831</v>
+        <v>45832</v>
       </c>
       <c r="B127" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="B128" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>45828</v>
+        <v>45829</v>
       </c>
       <c r="B129" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>45827</v>
+        <v>45828</v>
       </c>
       <c r="B130" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>45826</v>
+        <v>45827</v>
       </c>
       <c r="B131" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="B132" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>45824</v>
+        <v>45825</v>
       </c>
       <c r="B133" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>45822</v>
+        <v>45824</v>
       </c>
       <c r="B134" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>45821</v>
+        <v>45822</v>
       </c>
       <c r="B135" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>45820</v>
+        <v>45821</v>
       </c>
       <c r="B136" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>45819</v>
+        <v>45820</v>
       </c>
       <c r="B137" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>45818</v>
+        <v>45819</v>
       </c>
       <c r="B138" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="B139" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>45815</v>
+        <v>45817</v>
       </c>
       <c r="B140" t="n">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>45814</v>
+        <v>45815</v>
       </c>
       <c r="B141" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>45813</v>
+        <v>45814</v>
       </c>
       <c r="B142" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>45812</v>
+        <v>45813</v>
       </c>
       <c r="B143" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>45811</v>
+        <v>45812</v>
       </c>
       <c r="B144" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>45810</v>
+        <v>45811</v>
       </c>
       <c r="B145" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>45808</v>
+        <v>45810</v>
       </c>
       <c r="B146" t="n">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>45807</v>
+        <v>45808</v>
       </c>
       <c r="B147" t="n">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="B148" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>45805</v>
+        <v>45806</v>
       </c>
       <c r="B149" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>45804</v>
+        <v>45805</v>
       </c>
       <c r="B150" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>45803</v>
+        <v>45804</v>
       </c>
       <c r="B151" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>45801</v>
+        <v>45803</v>
       </c>
       <c r="B152" t="n">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>45800</v>
+        <v>45801</v>
       </c>
       <c r="B153" t="n">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>45799</v>
+        <v>45800</v>
       </c>
       <c r="B154" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>45798</v>
+        <v>45799</v>
       </c>
       <c r="B155" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>45797</v>
+        <v>45798</v>
       </c>
       <c r="B156" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>45796</v>
+        <v>45797</v>
       </c>
       <c r="B157" t="n">
         <v>41</v>
@@ -1699,31 +1699,31 @@
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>45793</v>
+        <v>45796</v>
       </c>
       <c r="B158" t="n">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>45792</v>
+        <v>45793</v>
       </c>
       <c r="B159" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45791</v>
+        <v>45792</v>
       </c>
       <c r="B160" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45790</v>
+        <v>45791</v>
       </c>
       <c r="B161" t="n">
         <v>35</v>
@@ -1731,65 +1731,73 @@
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>45789</v>
+        <v>45790</v>
       </c>
       <c r="B162" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>45786</v>
+        <v>45789</v>
       </c>
       <c r="B163" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>45785</v>
+        <v>45786</v>
       </c>
       <c r="B164" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
-        <v>45784</v>
+        <v>45785</v>
       </c>
       <c r="B165" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
-        <v>45783</v>
+        <v>45784</v>
       </c>
       <c r="B166" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
-        <v>45782</v>
+        <v>45783</v>
       </c>
       <c r="B167" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
-        <v>45779</v>
+        <v>45782</v>
       </c>
       <c r="B168" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
+        <v>45779</v>
+      </c>
+      <c r="B169" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
         <v>45778</v>
       </c>
-      <c r="B169" t="n">
+      <c r="B170" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>